<commit_message>
Doc: Added actual hours for UI Design
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEA8575-1765-4045-9871-6852706024CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE609C6-2FC4-4156-957E-9C9637352E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WP" sheetId="1" r:id="rId1"/>
@@ -773,26 +773,69 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,7 +869,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -834,51 +876,9 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1130,13 +1130,13 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="80"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1151,13 +1151,13 @@
       <c r="E2" s="7">
         <v>3</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="72"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1170,13 +1170,13 @@
       <c r="E3" s="7">
         <v>3</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="72"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1185,13 +1185,13 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="44"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
@@ -1200,13 +1200,13 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="44"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1215,13 +1215,13 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="44"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1230,13 +1230,13 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="44"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="58"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1247,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
@@ -1266,13 +1266,13 @@
       <c r="E9" s="7">
         <v>1</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="72"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1282,14 +1282,16 @@
       <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="43" t="s">
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
@@ -1302,13 +1304,13 @@
       <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="72"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1317,13 +1319,13 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1332,13 +1334,13 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1348,14 +1350,16 @@
       <c r="D14" s="7">
         <v>1</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="43" t="s">
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1366,13 +1370,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="58"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1383,13 +1387,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="5" t="s">
         <v>43</v>
       </c>
@@ -1400,13 +1404,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="44"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="58"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="5" t="s">
         <v>44</v>
       </c>
@@ -1416,14 +1420,16 @@
       <c r="D18" s="7">
         <v>0.5</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="44"/>
+      <c r="E18" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
@@ -1432,13 +1438,13 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="44"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="5" t="s">
         <v>46</v>
       </c>
@@ -1448,14 +1454,16 @@
       <c r="D20" s="7">
         <v>0.5</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="44"/>
+      <c r="E20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
@@ -1464,10 +1472,10 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="44"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
@@ -1475,11 +1483,11 @@
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="46"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="78" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1494,13 +1502,13 @@
       <c r="E23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="71" t="s">
+      <c r="F23" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="72"/>
+      <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="58"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1513,13 +1521,13 @@
       <c r="E24" s="7">
         <v>3</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="72"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="58"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1528,13 +1536,13 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="43" t="s">
+      <c r="F25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="58"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
@@ -1543,13 +1551,13 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="43" t="s">
+      <c r="F26" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="58"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
@@ -1558,13 +1566,13 @@
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="43" t="s">
+      <c r="F27" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="44"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="58"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
@@ -1573,13 +1581,13 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="43" t="s">
+      <c r="F28" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="44"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="58"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
@@ -1590,13 +1598,13 @@
         <v>3</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="44"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="58"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
@@ -1607,13 +1615,13 @@
         <v>3</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="43" t="s">
+      <c r="F30" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="44"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="58"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="5" t="s">
         <v>56</v>
       </c>
@@ -1624,13 +1632,13 @@
         <v>3</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="F31" s="43" t="s">
+      <c r="F31" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="44"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="58"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="5" t="s">
         <v>57</v>
       </c>
@@ -1641,13 +1649,13 @@
         <v>3</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="43" t="s">
+      <c r="F32" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="44"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="58"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="5" t="s">
         <v>58</v>
       </c>
@@ -1656,13 +1664,13 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="43" t="s">
+      <c r="F33" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="5" t="s">
         <v>59</v>
       </c>
@@ -1671,13 +1679,13 @@
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="43" t="s">
+      <c r="F34" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="44"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="5" t="s">
         <v>60</v>
       </c>
@@ -1688,13 +1696,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="43" t="s">
+      <c r="F35" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="44"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="58"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="5" t="s">
         <v>61</v>
       </c>
@@ -1705,13 +1713,13 @@
         <v>1</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="43" t="s">
+      <c r="F36" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="44"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="5" t="s">
         <v>62</v>
       </c>
@@ -1722,13 +1730,13 @@
         <v>1</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="44"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="5" t="s">
         <v>63</v>
       </c>
@@ -1739,13 +1747,13 @@
         <v>1</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="43" t="s">
+      <c r="F38" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="44"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="58"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
@@ -1756,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="44"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="58"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="5" t="s">
         <v>65</v>
       </c>
@@ -1771,13 +1779,13 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="43" t="s">
+      <c r="F40" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="44"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="58"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="5" t="s">
         <v>66</v>
       </c>
@@ -1788,13 +1796,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="7"/>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="44"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="59"/>
+      <c r="A42" s="77"/>
       <c r="B42" s="5" t="s">
         <v>67</v>
       </c>
@@ -1803,10 +1811,10 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="43" t="s">
+      <c r="F42" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="44"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
@@ -1814,64 +1822,64 @@
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="46"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="42"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="79" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="64"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="51"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="62"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="18"/>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="64"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="51"/>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="62"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="18"/>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="64"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="51"/>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="62"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="18"/>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="64"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="51"/>
     </row>
     <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="70"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
+      <c r="A49" s="80"/>
       <c r="B49" s="19"/>
       <c r="C49" s="20"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="70"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="53"/>
     </row>
     <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
@@ -1879,67 +1887,67 @@
       <c r="C50" s="15"/>
       <c r="D50" s="16"/>
       <c r="E50" s="17"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="46"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="67"/>
-      <c r="C51" s="67" t="s">
+      <c r="B51" s="49"/>
+      <c r="C51" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="73">
+      <c r="D51" s="54">
         <v>3</v>
       </c>
-      <c r="E51" s="76"/>
-      <c r="F51" s="47" t="s">
+      <c r="E51" s="57"/>
+      <c r="F51" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="48"/>
+      <c r="G51" s="67"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="77"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="50"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="69"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="58"/>
-      <c r="B53" s="68"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="50"/>
+      <c r="A53" s="44"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="69"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
-      <c r="B54" s="68"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="50"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="69"/>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="65"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="66"/>
+      <c r="A55" s="45"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="61"/>
       <c r="C56" s="33" t="s">
         <v>25</v>
       </c>
@@ -1949,14 +1957,14 @@
       <c r="E56" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="41" t="s">
+      <c r="F56" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G56" s="42"/>
+      <c r="G56" s="65"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37"/>
-      <c r="B57" s="38"/>
+      <c r="A57" s="62"/>
+      <c r="B57" s="47"/>
       <c r="C57" s="30" t="s">
         <v>23</v>
       </c>
@@ -1965,15 +1973,15 @@
         <f>(D57/D56)</f>
         <v>0</v>
       </c>
-      <c r="F57" s="51">
+      <c r="F57" s="70">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>14</v>
-      </c>
-      <c r="G57" s="52"/>
+        <v>18</v>
+      </c>
+      <c r="G57" s="71"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
-      <c r="B58" s="38"/>
+      <c r="A58" s="62"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="31" t="s">
         <v>24</v>
       </c>
@@ -1984,12 +1992,12 @@
         <f>D58/D56</f>
         <v>1</v>
       </c>
-      <c r="F58" s="53"/>
-      <c r="G58" s="54"/>
+      <c r="F58" s="72"/>
+      <c r="G58" s="73"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
-      <c r="B59" s="40"/>
+      <c r="A59" s="63"/>
+      <c r="B59" s="46"/>
       <c r="C59" s="32" t="s">
         <v>12</v>
       </c>
@@ -1998,8 +2006,8 @@
         <f>D59/D56</f>
         <v>0</v>
       </c>
-      <c r="F59" s="55"/>
-      <c r="G59" s="56"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="75"/>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="21"/>
@@ -5811,6 +5819,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A56:B59"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F51:G54"/>
+    <mergeCell ref="F57:G59"/>
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="A23:A42"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F1:G1"/>
@@ -5827,56 +5882,9 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A56:B59"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F51:G54"/>
-    <mergeCell ref="F57:G59"/>
-    <mergeCell ref="A2:A21"/>
-    <mergeCell ref="A23:A42"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F1:F21 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F23:F42 F44:F49 F61:G1012 F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5893,8 +5901,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5932,7 +5940,7 @@
       </c>
       <c r="D2" s="25">
         <f>WP!E9 + WP!E11 + WP!E18 + WP!E20 + WP!E30 + WP!E32 + WP!E39 + WP!E41  + WP!E51</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5948,7 +5956,7 @@
       </c>
       <c r="D3" s="25">
         <f>WP!E8 + WP!E10 + WP!E14 + WP!E16 + WP!E29 + WP!E31 + WP!E35 + WP!E37</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6009,7 +6017,7 @@
       </c>
       <c r="D7" s="26">
         <f>D2+D3+D4+D5+D6</f>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: Added actual hours for UI Design for cart and checkout and actual hours for backend for cart
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE609C6-2FC4-4156-957E-9C9637352E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAD9DBF-F584-4F49-B9DB-94292C469A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WP" sheetId="1" r:id="rId1"/>
@@ -773,12 +773,20 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,53 +797,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,6 +830,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -876,9 +838,47 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1130,13 +1130,13 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="80"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1151,13 +1151,13 @@
       <c r="E2" s="7">
         <v>3</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1170,13 +1170,13 @@
       <c r="E3" s="7">
         <v>3</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1185,28 +1185,32 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="36"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="36"/>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1215,28 +1219,32 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="36"/>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1247,13 +1255,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
@@ -1266,13 +1274,13 @@
       <c r="E9" s="7">
         <v>1</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="40"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1285,13 +1293,13 @@
       <c r="E10" s="7">
         <v>2</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
@@ -1304,43 +1312,47 @@
       <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="40"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1353,13 +1365,13 @@
       <c r="E14" s="7">
         <v>1</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1370,13 +1382,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="44"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1387,13 +1399,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="5" t="s">
         <v>43</v>
       </c>
@@ -1404,13 +1416,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="5" t="s">
         <v>44</v>
       </c>
@@ -1423,13 +1435,13 @@
       <c r="E18" s="7">
         <v>0.5</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="40"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="44"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
@@ -1438,13 +1450,13 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="44"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="5" t="s">
         <v>46</v>
       </c>
@@ -1457,13 +1469,13 @@
       <c r="E20" s="7">
         <v>0.5</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="40"/>
+      <c r="G20" s="46"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="77"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
@@ -1472,10 +1484,10 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
@@ -1483,11 +1495,11 @@
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1502,13 +1514,13 @@
       <c r="E23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="44"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1521,13 +1533,13 @@
       <c r="E24" s="7">
         <v>3</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="46"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1536,28 +1548,32 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="36"/>
+      <c r="G25" s="44"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="36"/>
+      <c r="D26" s="7">
+        <v>4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>4</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="46"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
@@ -1566,28 +1582,30 @@
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="44"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="44"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="7">
+        <v>4</v>
+      </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="44"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="44"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
@@ -1598,13 +1616,13 @@
         <v>3</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="44"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="44"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
@@ -1615,13 +1633,13 @@
         <v>3</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="36"/>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="44"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="5" t="s">
         <v>56</v>
       </c>
@@ -1632,13 +1650,13 @@
         <v>3</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="44"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="5" t="s">
         <v>57</v>
       </c>
@@ -1649,43 +1667,47 @@
         <v>3</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="36"/>
+      <c r="G32" s="44"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="44"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="35" t="s">
+      <c r="F33" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="36"/>
+      <c r="G33" s="44"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E34" s="7"/>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="36"/>
+      <c r="G34" s="44"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="44"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="5" t="s">
         <v>60</v>
       </c>
@@ -1696,13 +1718,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="36"/>
+      <c r="G35" s="44"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="44"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="5" t="s">
         <v>61</v>
       </c>
@@ -1713,13 +1735,13 @@
         <v>1</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="5" t="s">
         <v>62</v>
       </c>
@@ -1730,13 +1752,13 @@
         <v>1</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="36"/>
+      <c r="G37" s="44"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="44"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="5" t="s">
         <v>63</v>
       </c>
@@ -1747,13 +1769,13 @@
         <v>1</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="36"/>
+      <c r="G38" s="44"/>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="44"/>
+      <c r="A39" s="60"/>
       <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
@@ -1764,13 +1786,13 @@
         <v>1</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="36"/>
+      <c r="G39" s="44"/>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="44"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="5" t="s">
         <v>65</v>
       </c>
@@ -1779,13 +1801,13 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="36"/>
+      <c r="G40" s="44"/>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="44"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="5" t="s">
         <v>66</v>
       </c>
@@ -1796,13 +1818,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="7"/>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="36"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="77"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="5" t="s">
         <v>67</v>
       </c>
@@ -1811,10 +1833,10 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="36"/>
+      <c r="G42" s="44"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
@@ -1822,64 +1844,64 @@
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="79" t="s">
+      <c r="A44" s="63" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="51"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="70"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="43"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="18"/>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="51"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="70"/>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="43"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="18"/>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="51"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="70"/>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="43"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="18"/>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="51"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="70"/>
     </row>
     <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="72"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="80"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="19"/>
       <c r="C49" s="20"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="53"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="72"/>
     </row>
     <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
@@ -1887,67 +1909,67 @@
       <c r="C50" s="15"/>
       <c r="D50" s="16"/>
       <c r="E50" s="17"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49" t="s">
+      <c r="B51" s="68"/>
+      <c r="C51" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="54">
+      <c r="D51" s="73">
         <v>3</v>
       </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="66" t="s">
+      <c r="E51" s="76"/>
+      <c r="F51" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="67"/>
+      <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="44"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="69"/>
+      <c r="A52" s="60"/>
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="44"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="69"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="52"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="44"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="69"/>
+      <c r="A54" s="60"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="52"/>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="45"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="48"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="67"/>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="60" t="s">
+      <c r="A56" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="61"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="33" t="s">
         <v>25</v>
       </c>
@@ -1957,14 +1979,14 @@
       <c r="E56" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="64" t="s">
+      <c r="F56" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G56" s="65"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="62"/>
-      <c r="B57" s="47"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="30" t="s">
         <v>23</v>
       </c>
@@ -1973,15 +1995,15 @@
         <f>(D57/D56)</f>
         <v>0</v>
       </c>
-      <c r="F57" s="70">
+      <c r="F57" s="53">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>18</v>
-      </c>
-      <c r="G57" s="71"/>
+        <v>26</v>
+      </c>
+      <c r="G57" s="54"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="62"/>
-      <c r="B58" s="47"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="31" t="s">
         <v>24</v>
       </c>
@@ -1992,12 +2014,12 @@
         <f>D58/D56</f>
         <v>1</v>
       </c>
-      <c r="F58" s="72"/>
-      <c r="G58" s="73"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="56"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="63"/>
-      <c r="B59" s="46"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="32" t="s">
         <v>12</v>
       </c>
@@ -2006,8 +2028,8 @@
         <f>D59/D56</f>
         <v>0</v>
       </c>
-      <c r="F59" s="74"/>
-      <c r="G59" s="75"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="58"/>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="21"/>
@@ -5819,6 +5841,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
     <mergeCell ref="A56:B59"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F17:G17"/>
@@ -5835,56 +5904,9 @@
     <mergeCell ref="A23:A42"/>
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F23:F42 F44:F49 F61:G1012 F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F1:F21 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5901,8 +5923,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5993,14 +6015,16 @@
       <c r="A6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="25">
+        <v>15</v>
+      </c>
       <c r="C6" s="25">
         <f>WP!D5 + WP!D7 + WP!D12 + WP!D13 + WP!D26 + WP!D28 + WP!D33 + WP!D34</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D6" s="25">
         <f>WP!E5 + WP!E7 + WP!E12 + WP!E13 + WP!E26 + WP!E28 + WP!E33 + WP!E34</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6009,15 +6033,15 @@
       </c>
       <c r="B7" s="26">
         <f>B2+B3+B4+B5+B6</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C7" s="26">
         <f>C2+C3+C4+C5+C6</f>
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D7" s="26">
         <f>D2+D3+D4+D5+D6</f>
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: added actual hours for backend of supplier features
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9C8DF-A0DC-4F35-8932-18D332B5B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4B466B-C531-46EC-82F8-3993E6EE5CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,8 +1110,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1194,10 +1194,14 @@
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="39" t="s">
-        <v>24</v>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="34">
+        <v>2</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G4" s="37"/>
     </row>
@@ -1228,7 +1232,9 @@
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
       <c r="E6" s="34"/>
       <c r="F6" s="39" t="s">
         <v>24</v>
@@ -1265,9 +1271,11 @@
       <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="39" t="s">
-        <v>24</v>
+      <c r="E8" s="34">
+        <v>2</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G8" s="37"/>
     </row>
@@ -1304,8 +1312,8 @@
       <c r="E10" s="34">
         <v>2</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>24</v>
+      <c r="F10" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G10" s="37"/>
     </row>
@@ -1339,9 +1347,11 @@
       <c r="D12" s="6">
         <v>0.5</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="39" t="s">
-        <v>24</v>
+      <c r="E12" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G12" s="37"/>
     </row>
@@ -1356,9 +1366,11 @@
       <c r="D13" s="6">
         <v>0.5</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="39" t="s">
-        <v>24</v>
+      <c r="E13" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G13" s="37"/>
     </row>
@@ -1376,8 +1388,8 @@
       <c r="E14" s="34">
         <v>1</v>
       </c>
-      <c r="F14" s="39" t="s">
-        <v>24</v>
+      <c r="F14" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G14" s="37"/>
     </row>
@@ -1459,10 +1471,14 @@
       <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="39" t="s">
-        <v>24</v>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="34">
+        <v>1</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G19" s="37"/>
     </row>
@@ -1493,10 +1509,14 @@
       <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="39" t="s">
-        <v>24</v>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="34">
+        <v>1</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G21" s="37"/>
     </row>
@@ -1557,10 +1577,12 @@
       <c r="C25" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="6">
+        <v>4</v>
+      </c>
       <c r="E25" s="34"/>
-      <c r="F25" s="39" t="s">
-        <v>24</v>
+      <c r="F25" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="G25" s="37"/>
     </row>
@@ -1591,7 +1613,9 @@
       <c r="C27" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="6">
+        <v>4</v>
+      </c>
       <c r="E27" s="34"/>
       <c r="F27" s="39" t="s">
         <v>24</v>
@@ -1610,8 +1634,8 @@
         <v>4</v>
       </c>
       <c r="E28" s="34"/>
-      <c r="F28" s="39" t="s">
-        <v>24</v>
+      <c r="F28" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="G28" s="37"/>
     </row>
@@ -1626,9 +1650,11 @@
       <c r="D29" s="6">
         <v>3</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="44" t="s">
-        <v>23</v>
+      <c r="E29" s="34">
+        <v>3</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G29" s="37"/>
     </row>
@@ -1643,9 +1669,11 @@
       <c r="D30" s="6">
         <v>3</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="44" t="s">
-        <v>23</v>
+      <c r="E30" s="34">
+        <v>3</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G30" s="37"/>
     </row>
@@ -1660,9 +1688,11 @@
       <c r="D31" s="6">
         <v>3</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="44" t="s">
-        <v>23</v>
+      <c r="E31" s="34">
+        <v>3</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G31" s="37"/>
     </row>
@@ -1677,9 +1707,11 @@
       <c r="D32" s="6">
         <v>3</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="44" t="s">
-        <v>23</v>
+      <c r="E32" s="34">
+        <v>3</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G32" s="37"/>
     </row>
@@ -1694,9 +1726,11 @@
       <c r="D33" s="6">
         <v>0.5</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="39" t="s">
-        <v>24</v>
+      <c r="E33" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G33" s="37"/>
     </row>
@@ -1711,9 +1745,11 @@
       <c r="D34" s="6">
         <v>0.5</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="39" t="s">
-        <v>24</v>
+      <c r="E34" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G34" s="37"/>
     </row>
@@ -1796,9 +1832,11 @@
       <c r="D39" s="6">
         <v>1</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="39" t="s">
-        <v>24</v>
+      <c r="E39" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G39" s="37"/>
     </row>
@@ -1810,10 +1848,14 @@
       <c r="C40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="39" t="s">
-        <v>24</v>
+      <c r="D40" s="6">
+        <v>1</v>
+      </c>
+      <c r="E40" s="34">
+        <v>1</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G40" s="37"/>
     </row>
@@ -1828,9 +1870,11 @@
       <c r="D41" s="6">
         <v>1</v>
       </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="39" t="s">
-        <v>24</v>
+      <c r="E41" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G41" s="37"/>
     </row>
@@ -1842,10 +1886,14 @@
       <c r="C42" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="39" t="s">
-        <v>24</v>
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="34">
+        <v>1</v>
+      </c>
+      <c r="F42" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G42" s="37"/>
     </row>
@@ -2004,15 +2052,15 @@
       </c>
       <c r="D57" s="27">
         <f>COUNTIF(F2:F54,"Doing")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E57" s="26">
         <f>(D57/D56)</f>
-        <v>9.7560975609756101E-2</v>
+        <v>4.878048780487805E-2</v>
       </c>
       <c r="F57" s="53">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G57" s="54"/>
     </row>
@@ -2024,11 +2072,11 @@
       </c>
       <c r="D58" s="28">
         <f>COUNTIF(F2:F54,"To do")</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E58" s="26">
         <f>D58/D56</f>
-        <v>0.63414634146341464</v>
+        <v>0.24390243902439024</v>
       </c>
       <c r="F58" s="55"/>
       <c r="G58" s="56"/>
@@ -2041,11 +2089,11 @@
       </c>
       <c r="D59" s="29">
         <f>COUNTIF(F2:F54,"Done")</f>
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E59" s="26">
         <f>D59/D56</f>
-        <v>0.26829268292682928</v>
+        <v>0.70731707317073167</v>
       </c>
       <c r="F59" s="57"/>
       <c r="G59" s="58"/>
@@ -5874,7 +5922,7 @@
     <mergeCell ref="E51:E54"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F1:F21 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F23:F42 F44:F49 F61:G1012 F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5892,7 +5940,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5930,7 +5978,7 @@
       </c>
       <c r="D2" s="22">
         <f>WP!E9 + WP!E11 + WP!E18 + WP!E20 + WP!E30 + WP!E32 + WP!E39 + WP!E41  + WP!E51</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5946,7 +5994,7 @@
       </c>
       <c r="D3" s="22">
         <f>WP!E8 + WP!E10 + WP!E14 + WP!E16 + WP!E29 + WP!E31 + WP!E35 + WP!E37</f>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5969,14 +6017,16 @@
       <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="22">
+        <v>14</v>
+      </c>
       <c r="C5" s="22">
         <f>WP!D4 + WP!D6 + WP!D19 + WP!D21 + WP!D25 + WP!D27 + WP!D40 + WP!D42</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D5" s="22">
         <f>WP!E4 + WP!E6 + WP!E19 + WP!E21 + WP!E25 + WP!E27 + WP!E40 + WP!E42</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5992,7 +6042,7 @@
       </c>
       <c r="D6" s="22">
         <f>WP!E5 + WP!E7 + WP!E12 + WP!E13 + WP!E26 + WP!E28 + WP!E33 + WP!E34</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6001,15 +6051,15 @@
       </c>
       <c r="B7" s="23">
         <f>B2+B3+B4+B5+B6</f>
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C7" s="23">
         <f>C2+C3+C4+C5+C6</f>
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D7" s="23">
         <f>D2+D3+D4+D5+D6</f>
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: added actual hours for frontend and backend of client home page
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4B466B-C531-46EC-82F8-3993E6EE5CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8DA98D-1D72-473C-BBB3-33B53D91B62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,8 +1110,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1580,9 +1580,11 @@
       <c r="D25" s="6">
         <v>4</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="44" t="s">
-        <v>23</v>
+      <c r="E25" s="34">
+        <v>5</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G25" s="37"/>
     </row>
@@ -1764,9 +1766,11 @@
       <c r="D35" s="6">
         <v>1</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="39" t="s">
-        <v>24</v>
+      <c r="E35" s="34">
+        <v>1</v>
+      </c>
+      <c r="F35" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G35" s="37"/>
     </row>
@@ -2052,15 +2056,15 @@
       </c>
       <c r="D57" s="27">
         <f>COUNTIF(F2:F54,"Doing")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" s="26">
         <f>(D57/D56)</f>
-        <v>4.878048780487805E-2</v>
+        <v>2.4390243902439025E-2</v>
       </c>
       <c r="F57" s="53">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G57" s="54"/>
     </row>
@@ -2072,11 +2076,11 @@
       </c>
       <c r="D58" s="28">
         <f>COUNTIF(F2:F54,"To do")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58" s="26">
         <f>D58/D56</f>
-        <v>0.24390243902439024</v>
+        <v>0.21951219512195122</v>
       </c>
       <c r="F58" s="55"/>
       <c r="G58" s="56"/>
@@ -2089,11 +2093,11 @@
       </c>
       <c r="D59" s="29">
         <f>COUNTIF(F2:F54,"Done")</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E59" s="26">
         <f>D59/D56</f>
-        <v>0.70731707317073167</v>
+        <v>0.75609756097560976</v>
       </c>
       <c r="F59" s="57"/>
       <c r="G59" s="58"/>
@@ -5922,7 +5926,7 @@
     <mergeCell ref="E51:E54"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F23:F42 F44:F49 F61:G1012 F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F1:F21 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5994,7 +5998,7 @@
       </c>
       <c r="D3" s="22">
         <f>WP!E8 + WP!E10 + WP!E14 + WP!E16 + WP!E29 + WP!E31 + WP!E35 + WP!E37</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6026,7 +6030,7 @@
       </c>
       <c r="D5" s="22">
         <f>WP!E4 + WP!E6 + WP!E19 + WP!E21 + WP!E25 + WP!E27 + WP!E40 + WP!E42</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6059,7 +6063,7 @@
       </c>
       <c r="D7" s="23">
         <f>D2+D3+D4+D5+D6</f>
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: added actual hours backend of cart page and Release 5 planning
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8DA98D-1D72-473C-BBB3-33B53D91B62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86ADD9C-D822-4B44-AD0C-8B56948FA082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -370,7 +370,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,14 +443,8 @@
         <bgColor rgb="FF4285F4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -708,11 +702,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -817,9 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,13 +896,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,8 +1134,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1147,7 +1171,7 @@
       <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="58" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1168,7 +1192,7 @@
       <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1211,7 @@
       <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1230,7 @@
       <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
@@ -1225,7 +1249,7 @@
       <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
@@ -1242,7 +1266,7 @@
       <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1261,7 +1285,7 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1304,7 @@
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="60"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1299,7 +1323,7 @@
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
@@ -1318,7 +1342,7 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="60"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1337,7 +1361,7 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="60"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
@@ -1356,7 +1380,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1399,7 @@
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
@@ -1394,7 +1418,7 @@
       <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -1404,14 +1428,16 @@
       <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="39" t="s">
-        <v>24</v>
+      <c r="E15" s="34">
+        <v>1</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="60"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1428,7 +1454,7 @@
       <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1445,7 +1471,7 @@
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1464,7 +1490,7 @@
       <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
@@ -1483,7 +1509,7 @@
       <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
@@ -1502,7 +1528,7 @@
       <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1530,7 +1556,7 @@
       <c r="G22" s="42"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="61" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1551,7 +1577,7 @@
       <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="4" t="s">
         <v>49</v>
       </c>
@@ -1570,7 +1596,7 @@
       <c r="G24" s="37"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
@@ -1589,7 +1615,7 @@
       <c r="G25" s="37"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
@@ -1608,7 +1634,7 @@
       <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="60"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="4" t="s">
         <v>52</v>
       </c>
@@ -1625,7 +1651,7 @@
       <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="4" t="s">
         <v>53</v>
       </c>
@@ -1636,13 +1662,13 @@
         <v>4</v>
       </c>
       <c r="E28" s="34"/>
-      <c r="F28" s="44" t="s">
-        <v>23</v>
+      <c r="F28" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="G28" s="37"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="60"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="4" t="s">
         <v>54</v>
       </c>
@@ -1661,7 +1687,7 @@
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
@@ -1680,7 +1706,7 @@
       <c r="G30" s="37"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
@@ -1699,7 +1725,7 @@
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="4" t="s">
         <v>57</v>
       </c>
@@ -1718,7 +1744,7 @@
       <c r="G32" s="37"/>
     </row>
     <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="60"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="4" t="s">
         <v>58</v>
       </c>
@@ -1737,7 +1763,7 @@
       <c r="G33" s="37"/>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="60"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="4" t="s">
         <v>59</v>
       </c>
@@ -1756,7 +1782,7 @@
       <c r="G34" s="37"/>
     </row>
     <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="4" t="s">
         <v>60</v>
       </c>
@@ -1775,7 +1801,7 @@
       <c r="G35" s="37"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="4" t="s">
         <v>61</v>
       </c>
@@ -1785,14 +1811,16 @@
       <c r="D36" s="6">
         <v>1</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="39" t="s">
-        <v>24</v>
+      <c r="E36" s="34">
+        <v>1</v>
+      </c>
+      <c r="F36" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G36" s="37"/>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="4" t="s">
         <v>62</v>
       </c>
@@ -1809,7 +1837,7 @@
       <c r="G37" s="37"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="4" t="s">
         <v>63</v>
       </c>
@@ -1826,7 +1854,7 @@
       <c r="G38" s="37"/>
     </row>
     <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="4" t="s">
         <v>64</v>
       </c>
@@ -1845,7 +1873,7 @@
       <c r="G39" s="37"/>
     </row>
     <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="60"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="4" t="s">
         <v>65</v>
       </c>
@@ -1864,7 +1892,7 @@
       <c r="G40" s="37"/>
     </row>
     <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="60"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="4" t="s">
         <v>66</v>
       </c>
@@ -1883,7 +1911,7 @@
       <c r="G41" s="37"/>
     </row>
     <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="61"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="4" t="s">
         <v>67</v>
       </c>
@@ -1911,7 +1939,7 @@
       <c r="G43" s="42"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="63" t="s">
+      <c r="A44" s="62" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="15"/>
@@ -1922,7 +1950,7 @@
       <c r="G44" s="37"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="64"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="15"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
@@ -1931,7 +1959,7 @@
       <c r="G45" s="37"/>
     </row>
     <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="64"/>
+      <c r="A46" s="63"/>
       <c r="B46" s="15"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -1940,7 +1968,7 @@
       <c r="G46" s="37"/>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="64"/>
+      <c r="A47" s="63"/>
       <c r="B47" s="15"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
@@ -1949,7 +1977,7 @@
       <c r="G47" s="37"/>
     </row>
     <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="64"/>
+      <c r="A48" s="63"/>
       <c r="B48" s="16"/>
       <c r="C48" s="17"/>
       <c r="D48" s="6"/>
@@ -1958,7 +1986,7 @@
       <c r="G48" s="37"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="65"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="16"/>
       <c r="C49" s="17"/>
       <c r="D49" s="6"/>
@@ -1976,63 +2004,65 @@
       <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="64" t="s">
+      <c r="A51" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="68"/>
-      <c r="C51" s="68" t="s">
+      <c r="B51" s="67"/>
+      <c r="C51" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="70">
+      <c r="D51" s="69">
         <v>3</v>
       </c>
-      <c r="E51" s="73"/>
-      <c r="F51" s="39" t="s">
-        <v>24</v>
+      <c r="E51" s="72">
+        <v>3</v>
+      </c>
+      <c r="F51" s="75" t="s">
+        <v>12</v>
       </c>
       <c r="G51" s="37"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="71"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="39"/>
+      <c r="A52" s="59"/>
+      <c r="B52" s="68"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="76"/>
       <c r="G52" s="37"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="71"/>
-      <c r="E53" s="74"/>
-      <c r="F53" s="39"/>
+      <c r="A53" s="59"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="76"/>
       <c r="G53" s="37"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="69"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="39"/>
+      <c r="A54" s="59"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="77"/>
       <c r="G54" s="37"/>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="66"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="67"/>
+      <c r="A55" s="65"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="66"/>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="46"/>
+      <c r="B56" s="45"/>
       <c r="C56" s="30" t="s">
         <v>25</v>
       </c>
@@ -2043,64 +2073,64 @@
       <c r="E56" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="51" t="s">
+      <c r="F56" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G56" s="52"/>
+      <c r="G56" s="51"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
-      <c r="B57" s="48"/>
+      <c r="A57" s="46"/>
+      <c r="B57" s="47"/>
       <c r="C57" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="27">
         <f>COUNTIF(F2:F54,"Doing")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="26">
         <f>(D57/D56)</f>
-        <v>2.4390243902439025E-2</v>
-      </c>
-      <c r="F57" s="53">
+        <v>0</v>
+      </c>
+      <c r="F57" s="52">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>55</v>
-      </c>
-      <c r="G57" s="54"/>
+        <v>60</v>
+      </c>
+      <c r="G57" s="53"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
-      <c r="B58" s="48"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D58" s="28">
         <f>COUNTIF(F2:F54,"To do")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E58" s="26">
         <f>D58/D56</f>
-        <v>0.21951219512195122</v>
-      </c>
-      <c r="F58" s="55"/>
-      <c r="G58" s="56"/>
+        <v>0.17073170731707318</v>
+      </c>
+      <c r="F58" s="54"/>
+      <c r="G58" s="55"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="49"/>
-      <c r="B59" s="50"/>
+      <c r="A59" s="48"/>
+      <c r="B59" s="49"/>
       <c r="C59" s="29" t="s">
         <v>12</v>
       </c>
       <c r="D59" s="29">
         <f>COUNTIF(F2:F54,"Done")</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E59" s="26">
         <f>D59/D56</f>
-        <v>0.75609756097560976</v>
-      </c>
-      <c r="F59" s="57"/>
-      <c r="G59" s="58"/>
+        <v>0.82926829268292679</v>
+      </c>
+      <c r="F59" s="56"/>
+      <c r="G59" s="57"/>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F61" s="18"/>
@@ -5911,7 +5941,7 @@
       <c r="G1012" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A56:B59"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F57:G59"/>
@@ -5924,9 +5954,10 @@
     <mergeCell ref="C51:C54"/>
     <mergeCell ref="D51:D54"/>
     <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F51:F54"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F51 F1:F21 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F21 F51 F44:F49 F61:G1012 F23:F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>" Doing,Done,To do"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5944,7 +5975,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5982,7 +6013,7 @@
       </c>
       <c r="D2" s="22">
         <f>WP!E9 + WP!E11 + WP!E18 + WP!E20 + WP!E30 + WP!E32 + WP!E39 + WP!E41  + WP!E51</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6014,7 +6045,7 @@
       </c>
       <c r="D4" s="22">
         <f>WP!E2 + WP!E3 + WP!E15 + WP!E17 + WP!E23 + WP!E24 + WP!E36 + WP!E38</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6022,7 +6053,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="22">
         <f>WP!D4 + WP!D6 + WP!D19 + WP!D21 + WP!D25 + WP!D27 + WP!D40 + WP!D42</f>
@@ -6055,7 +6086,7 @@
       </c>
       <c r="B7" s="23">
         <f>B2+B3+B4+B5+B6</f>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="23">
         <f>C2+C3+C4+C5+C6</f>
@@ -6063,7 +6094,7 @@
       </c>
       <c r="D7" s="23">
         <f>D2+D3+D4+D5+D6</f>
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: Updated Actual hours for checkout feature
</commit_message>
<xml_diff>
--- a/Release Planning/Release4_ planning.xlsx
+++ b/Release Planning/Release4_ planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Release Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86ADD9C-D822-4B44-AD0C-8B56948FA082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DD42EA-F328-4BD2-A3F8-842AC0C58232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,8 +1134,8 @@
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1259,9 +1259,11 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="39" t="s">
-        <v>24</v>
+      <c r="E6" s="34">
+        <v>2</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G6" s="37"/>
     </row>
@@ -1447,9 +1449,11 @@
       <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="39" t="s">
-        <v>24</v>
+      <c r="E16" s="34">
+        <v>1</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G16" s="37"/>
     </row>
@@ -1464,9 +1468,11 @@
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="39" t="s">
-        <v>24</v>
+      <c r="E17" s="34">
+        <v>1</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G17" s="37"/>
     </row>
@@ -1644,9 +1650,11 @@
       <c r="D27" s="6">
         <v>4</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="39" t="s">
-        <v>24</v>
+      <c r="E27" s="34">
+        <v>4</v>
+      </c>
+      <c r="F27" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G27" s="37"/>
     </row>
@@ -1830,9 +1838,11 @@
       <c r="D37" s="6">
         <v>1</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="39" t="s">
-        <v>24</v>
+      <c r="E37" s="34">
+        <v>1</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="G37" s="37"/>
     </row>
@@ -2094,7 +2104,7 @@
       </c>
       <c r="F57" s="52">
         <f>'Time Sheet'!D2 + 'Time Sheet'!D3 + 'Time Sheet'!D4 + 'Time Sheet'!D5 + 'Time Sheet'!D6</f>
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G57" s="53"/>
     </row>
@@ -2106,11 +2116,11 @@
       </c>
       <c r="D58" s="28">
         <f>COUNTIF(F2:F54,"To do")</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E58" s="26">
         <f>D58/D56</f>
-        <v>0.17073170731707318</v>
+        <v>4.878048780487805E-2</v>
       </c>
       <c r="F58" s="54"/>
       <c r="G58" s="55"/>
@@ -2123,11 +2133,11 @@
       </c>
       <c r="D59" s="29">
         <f>COUNTIF(F2:F54,"Done")</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E59" s="26">
         <f>D59/D56</f>
-        <v>0.82926829268292679</v>
+        <v>0.95121951219512191</v>
       </c>
       <c r="F59" s="56"/>
       <c r="G59" s="57"/>
@@ -6029,7 +6039,7 @@
       </c>
       <c r="D3" s="22">
         <f>WP!E8 + WP!E10 + WP!E14 + WP!E16 + WP!E29 + WP!E31 + WP!E35 + WP!E37</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6045,7 +6055,7 @@
       </c>
       <c r="D4" s="22">
         <f>WP!E2 + WP!E3 + WP!E15 + WP!E17 + WP!E23 + WP!E24 + WP!E36 + WP!E38</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6061,7 +6071,7 @@
       </c>
       <c r="D5" s="22">
         <f>WP!E4 + WP!E6 + WP!E19 + WP!E21 + WP!E25 + WP!E27 + WP!E40 + WP!E42</f>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6094,7 +6104,7 @@
       </c>
       <c r="D7" s="23">
         <f>D2+D3+D4+D5+D6</f>
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>